<commit_message>
Added sprite palette offset calculation (needs verification)
</commit_message>
<xml_diff>
--- a/Docs/Other/sprite_bounds_check.xlsx
+++ b/Docs/Other/sprite_bounds_check.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1453924358A\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\JCAP\Docs\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>temp</t>
   </si>
@@ -108,13 +108,40 @@
   </si>
   <si>
     <t>c ? : (cursl &lt; temp+1) ? &amp; c</t>
+  </si>
+  <si>
+    <t>temp:</t>
+  </si>
+  <si>
+    <t>tgt:</t>
+  </si>
+  <si>
+    <t>VERTICAL</t>
+  </si>
+  <si>
+    <t>HORIZONTAL</t>
+  </si>
+  <si>
+    <t>offset = spxsz - temp - 1</t>
+  </si>
+  <si>
+    <t>offset = spysz - (temp - cursl) - 1</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>cursl</t>
+  </si>
+  <si>
+    <t>offset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +149,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +184,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -219,11 +267,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -245,6 +319,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +643,7 @@
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -574,8 +653,14 @@
       <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>162</v>
       </c>
@@ -591,8 +676,16 @@
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>163</v>
       </c>
@@ -608,8 +701,15 @@
       <c r="E3" s="5">
         <v>249</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>164</v>
       </c>
@@ -625,8 +725,15 @@
       <c r="E4" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>165</v>
       </c>
@@ -642,8 +749,18 @@
       <c r="E5" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>166</v>
       </c>
@@ -653,8 +770,23 @@
       <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="13"/>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>167</v>
       </c>
@@ -664,8 +796,21 @@
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>168</v>
       </c>
@@ -675,8 +820,21 @@
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>169</v>
       </c>
@@ -686,8 +844,11 @@
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>170</v>
       </c>
@@ -697,8 +858,19 @@
       <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -708,8 +880,14 @@
       <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -725,8 +903,17 @@
       <c r="E13" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
@@ -742,8 +929,21 @@
       <c r="E14" s="5">
         <v>505</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="L14" s="11"/>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>17</v>
       </c>
@@ -759,8 +959,15 @@
       <c r="E15" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -770,8 +977,18 @@
       <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
@@ -781,8 +998,15 @@
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>17</v>
       </c>
@@ -792,8 +1016,15 @@
       <c r="C18" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
@@ -803,8 +1034,28 @@
       <c r="C19" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>255</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added tilemap position variables; refactored render system variable loading; implemented explicit scanline sprite limit
</commit_message>
<xml_diff>
--- a/Docs/Other/sprite_bounds_check.xlsx
+++ b/Docs/Other/sprite_bounds_check.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>temp</t>
   </si>
@@ -174,6 +174,36 @@
   </si>
   <si>
     <t>%11111111_11111111_11111111_00000000</t>
+  </si>
+  <si>
+    <t>LONG 0</t>
+  </si>
+  <si>
+    <t>LONG 1</t>
+  </si>
+  <si>
+    <t>TILE 0</t>
+  </si>
+  <si>
+    <t>TILE 1</t>
+  </si>
+  <si>
+    <t>TILE 2</t>
+  </si>
+  <si>
+    <t>TILE 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIXEL: </t>
+  </si>
+  <si>
+    <t>X POSITION:</t>
+  </si>
+  <si>
+    <t>x pos:</t>
+  </si>
+  <si>
+    <t>Parse part of tile A then jump back to parse part of tile B?</t>
   </si>
 </sst>
 </file>
@@ -198,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +277,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,11 +401,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -390,9 +443,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,6 +450,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -733,19 +810,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1135,64 +1212,64 @@
       <c r="C26" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="19">
-        <v>0</v>
-      </c>
-      <c r="E26" s="19">
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
+      <c r="E26" s="18">
         <v>1</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="18">
         <v>2</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="18">
         <v>3</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="18">
         <v>4</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="18">
         <v>5</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="18">
         <v>6</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="18">
         <v>7</v>
       </c>
-      <c r="L26" s="19">
+      <c r="L26" s="18">
         <v>8</v>
       </c>
-      <c r="M26" s="19">
+      <c r="M26" s="18">
         <v>9</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="18">
         <v>10</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="18">
         <v>11</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="18">
         <v>12</v>
       </c>
-      <c r="Q26" s="19">
+      <c r="Q26" s="18">
         <v>13</v>
       </c>
-      <c r="R26" s="19">
+      <c r="R26" s="18">
         <v>14</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="18">
         <v>15</v>
       </c>
-      <c r="T26" s="19">
+      <c r="T26" s="18">
         <v>16</v>
       </c>
-      <c r="U26" s="19">
+      <c r="U26" s="18">
         <v>17</v>
       </c>
-      <c r="V26" s="19">
+      <c r="V26" s="18">
         <v>18</v>
       </c>
-      <c r="W26" s="19">
+      <c r="W26" s="18">
         <v>19</v>
       </c>
     </row>
@@ -1200,99 +1277,99 @@
       <c r="C27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16" t="s">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16" t="s">
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16" t="s">
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16" t="s">
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C28" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <v>3</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="16">
         <v>2</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="16">
         <v>1</v>
       </c>
-      <c r="G28" s="17">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18">
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+      <c r="H28" s="17">
         <v>3</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="17">
         <v>2</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="17">
         <v>1</v>
       </c>
-      <c r="K28" s="18">
-        <v>0</v>
-      </c>
-      <c r="L28" s="17">
+      <c r="K28" s="17">
+        <v>0</v>
+      </c>
+      <c r="L28" s="16">
         <v>3</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M28" s="16">
         <v>2</v>
       </c>
-      <c r="N28" s="17">
+      <c r="N28" s="16">
         <v>1</v>
       </c>
-      <c r="O28" s="17">
-        <v>0</v>
-      </c>
-      <c r="P28" s="18">
+      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="P28" s="17">
         <v>3</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="Q28" s="17">
         <v>2</v>
       </c>
-      <c r="R28" s="18">
+      <c r="R28" s="17">
         <v>1</v>
       </c>
-      <c r="S28" s="18">
-        <v>0</v>
-      </c>
-      <c r="T28" s="17">
+      <c r="S28" s="17">
+        <v>0</v>
+      </c>
+      <c r="T28" s="16">
         <v>3</v>
       </c>
-      <c r="U28" s="17">
+      <c r="U28" s="16">
         <v>2</v>
       </c>
-      <c r="V28" s="17">
+      <c r="V28" s="16">
         <v>1</v>
       </c>
-      <c r="W28" s="17">
+      <c r="W28" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1341,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>7</v>
       </c>
@@ -1358,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>6</v>
       </c>
@@ -1375,7 +1452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>5</v>
       </c>
@@ -1392,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>4</v>
       </c>
@@ -1409,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>3</v>
       </c>
@@ -1426,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>2</v>
       </c>
@@ -1443,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>1</v>
       </c>
@@ -1460,8 +1537,326 @@
         <v>2</v>
       </c>
     </row>
+    <row r="42" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="27"/>
+      <c r="AB43" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="26"/>
+      <c r="AE43" s="26"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="26"/>
+      <c r="AH43" s="26"/>
+      <c r="AI43" s="27"/>
+    </row>
+    <row r="44" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y44" s="21"/>
+      <c r="Z44" s="21"/>
+      <c r="AA44" s="22"/>
+      <c r="AB44" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC44" s="21"/>
+      <c r="AD44" s="21"/>
+      <c r="AE44" s="22"/>
+      <c r="AF44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG44" s="21"/>
+      <c r="AH44" s="21"/>
+      <c r="AI44" s="22"/>
+    </row>
+    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="23">
+        <v>0</v>
+      </c>
+      <c r="E45" s="23">
+        <v>1</v>
+      </c>
+      <c r="F45" s="23">
+        <v>2</v>
+      </c>
+      <c r="G45" s="23">
+        <v>3</v>
+      </c>
+      <c r="H45" s="24">
+        <v>4</v>
+      </c>
+      <c r="I45" s="24">
+        <v>5</v>
+      </c>
+      <c r="J45" s="24">
+        <v>6</v>
+      </c>
+      <c r="K45" s="24">
+        <v>7</v>
+      </c>
+      <c r="L45" s="23">
+        <v>0</v>
+      </c>
+      <c r="M45" s="23">
+        <v>1</v>
+      </c>
+      <c r="N45" s="23">
+        <v>2</v>
+      </c>
+      <c r="O45" s="23">
+        <v>3</v>
+      </c>
+      <c r="P45" s="24">
+        <v>4</v>
+      </c>
+      <c r="Q45" s="24">
+        <v>5</v>
+      </c>
+      <c r="R45" s="24">
+        <v>6</v>
+      </c>
+      <c r="S45" s="24">
+        <v>7</v>
+      </c>
+      <c r="T45" s="23">
+        <v>0</v>
+      </c>
+      <c r="U45" s="23">
+        <v>1</v>
+      </c>
+      <c r="V45" s="23">
+        <v>2</v>
+      </c>
+      <c r="W45" s="23">
+        <v>3</v>
+      </c>
+      <c r="X45" s="24">
+        <v>4</v>
+      </c>
+      <c r="Y45" s="24">
+        <v>5</v>
+      </c>
+      <c r="Z45" s="24">
+        <v>6</v>
+      </c>
+      <c r="AA45" s="24">
+        <v>7</v>
+      </c>
+      <c r="AB45" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="23">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="23">
+        <v>2</v>
+      </c>
+      <c r="AE45" s="23">
+        <v>3</v>
+      </c>
+      <c r="AF45" s="24">
+        <v>4</v>
+      </c>
+      <c r="AG45" s="24">
+        <v>5</v>
+      </c>
+      <c r="AH45" s="24">
+        <v>6</v>
+      </c>
+      <c r="AI45" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C46" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
+        <v>2</v>
+      </c>
+      <c r="G46" s="9">
+        <v>3</v>
+      </c>
+      <c r="H46" s="9">
+        <v>4</v>
+      </c>
+      <c r="I46" s="9">
+        <v>5</v>
+      </c>
+      <c r="J46" s="9">
+        <v>6</v>
+      </c>
+      <c r="K46" s="9">
+        <v>7</v>
+      </c>
+      <c r="L46" s="9">
+        <v>8</v>
+      </c>
+      <c r="M46" s="9">
+        <v>9</v>
+      </c>
+      <c r="N46" s="9">
+        <v>10</v>
+      </c>
+      <c r="O46" s="9">
+        <v>11</v>
+      </c>
+      <c r="P46" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q46" s="9">
+        <v>13</v>
+      </c>
+      <c r="R46" s="9">
+        <v>14</v>
+      </c>
+      <c r="S46" s="9">
+        <v>15</v>
+      </c>
+      <c r="T46" s="9">
+        <v>16</v>
+      </c>
+      <c r="U46" s="9">
+        <v>17</v>
+      </c>
+      <c r="V46" s="9">
+        <v>18</v>
+      </c>
+      <c r="W46" s="9">
+        <v>19</v>
+      </c>
+      <c r="X46" s="9">
+        <v>20</v>
+      </c>
+      <c r="Y46" s="9">
+        <v>21</v>
+      </c>
+      <c r="Z46" s="9">
+        <v>22</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>23</v>
+      </c>
+      <c r="AB46" s="9">
+        <v>24</v>
+      </c>
+      <c r="AC46" s="9">
+        <v>25</v>
+      </c>
+      <c r="AD46" s="9">
+        <v>26</v>
+      </c>
+      <c r="AE46" s="9">
+        <v>27</v>
+      </c>
+      <c r="AF46" s="9">
+        <v>28</v>
+      </c>
+      <c r="AG46" s="9">
+        <v>29</v>
+      </c>
+      <c r="AH46" s="9">
+        <v>30</v>
+      </c>
+      <c r="AI46" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>58</v>
+      </c>
+      <c r="M48">
+        <v>14</v>
+      </c>
+      <c r="P48" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="17">
+    <mergeCell ref="AB43:AI43"/>
+    <mergeCell ref="AB44:AE44"/>
+    <mergeCell ref="AF44:AI44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="L43:S43"/>
+    <mergeCell ref="T43:AA43"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:W44"/>
+    <mergeCell ref="X44:AA44"/>
     <mergeCell ref="D27:G27"/>
     <mergeCell ref="H27:K27"/>
     <mergeCell ref="L27:O27"/>

</xml_diff>

<commit_message>
Removed sprite sizing from render routine
</commit_message>
<xml_diff>
--- a/Docs/Other/sprite_bounds_check.xlsx
+++ b/Docs/Other/sprite_bounds_check.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="25200" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="25200" windowHeight="11775" tabRatio="406"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>temp</t>
   </si>
@@ -200,10 +200,13 @@
     <t>X POSITION:</t>
   </si>
   <si>
-    <t>x pos:</t>
-  </si>
-  <si>
-    <t>Parse part of tile A then jump back to parse part of tile B?</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x/8</t>
+  </si>
+  <si>
+    <t>x%8</t>
   </si>
 </sst>
 </file>
@@ -452,18 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,6 +468,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI48"/>
+  <dimension ref="A1:AI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X58" sqref="X58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,36 +1280,36 @@
       <c r="C27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19" t="s">
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19" t="s">
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19" t="s">
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19" t="s">
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="W27" s="19"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C28" s="10" t="s">
@@ -1539,195 +1542,195 @@
     </row>
     <row r="42" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="25" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
-      <c r="Q43" s="26"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="25" t="s">
+      <c r="M43" s="22"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="U43" s="26"/>
-      <c r="V43" s="26"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="26"/>
-      <c r="Z43" s="26"/>
-      <c r="AA43" s="27"/>
-      <c r="AB43" s="25" t="s">
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
+      <c r="Z43" s="22"/>
+      <c r="AA43" s="23"/>
+      <c r="AB43" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AC43" s="26"/>
-      <c r="AD43" s="26"/>
-      <c r="AE43" s="26"/>
-      <c r="AF43" s="26"/>
-      <c r="AG43" s="26"/>
-      <c r="AH43" s="26"/>
-      <c r="AI43" s="27"/>
+      <c r="AC43" s="22"/>
+      <c r="AD43" s="22"/>
+      <c r="AE43" s="22"/>
+      <c r="AF43" s="22"/>
+      <c r="AG43" s="22"/>
+      <c r="AH43" s="22"/>
+      <c r="AI43" s="23"/>
     </row>
     <row r="44" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="20" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="20" t="s">
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="20" t="s">
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="Q44" s="21"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="20" t="s">
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="20" t="s">
+      <c r="U44" s="25"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="Y44" s="21"/>
-      <c r="Z44" s="21"/>
-      <c r="AA44" s="22"/>
-      <c r="AB44" s="20" t="s">
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AC44" s="21"/>
-      <c r="AD44" s="21"/>
-      <c r="AE44" s="22"/>
-      <c r="AF44" s="20" t="s">
+      <c r="AC44" s="25"/>
+      <c r="AD44" s="25"/>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AG44" s="21"/>
-      <c r="AH44" s="21"/>
-      <c r="AI44" s="22"/>
+      <c r="AG44" s="25"/>
+      <c r="AH44" s="25"/>
+      <c r="AI44" s="26"/>
     </row>
     <row r="45" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C45" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="23">
-        <v>0</v>
-      </c>
-      <c r="E45" s="23">
+      <c r="D45" s="19">
+        <v>0</v>
+      </c>
+      <c r="E45" s="19">
         <v>1</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="19">
         <v>2</v>
       </c>
-      <c r="G45" s="23">
+      <c r="G45" s="19">
         <v>3</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H45" s="20">
         <v>4</v>
       </c>
-      <c r="I45" s="24">
+      <c r="I45" s="20">
         <v>5</v>
       </c>
-      <c r="J45" s="24">
+      <c r="J45" s="20">
         <v>6</v>
       </c>
-      <c r="K45" s="24">
+      <c r="K45" s="20">
         <v>7</v>
       </c>
-      <c r="L45" s="23">
-        <v>0</v>
-      </c>
-      <c r="M45" s="23">
+      <c r="L45" s="19">
+        <v>0</v>
+      </c>
+      <c r="M45" s="19">
         <v>1</v>
       </c>
-      <c r="N45" s="23">
+      <c r="N45" s="19">
         <v>2</v>
       </c>
-      <c r="O45" s="23">
+      <c r="O45" s="19">
         <v>3</v>
       </c>
-      <c r="P45" s="24">
+      <c r="P45" s="20">
         <v>4</v>
       </c>
-      <c r="Q45" s="24">
+      <c r="Q45" s="20">
         <v>5</v>
       </c>
-      <c r="R45" s="24">
+      <c r="R45" s="20">
         <v>6</v>
       </c>
-      <c r="S45" s="24">
+      <c r="S45" s="20">
         <v>7</v>
       </c>
-      <c r="T45" s="23">
-        <v>0</v>
-      </c>
-      <c r="U45" s="23">
+      <c r="T45" s="19">
+        <v>0</v>
+      </c>
+      <c r="U45" s="19">
         <v>1</v>
       </c>
-      <c r="V45" s="23">
+      <c r="V45" s="19">
         <v>2</v>
       </c>
-      <c r="W45" s="23">
+      <c r="W45" s="19">
         <v>3</v>
       </c>
-      <c r="X45" s="24">
+      <c r="X45" s="20">
         <v>4</v>
       </c>
-      <c r="Y45" s="24">
+      <c r="Y45" s="20">
         <v>5</v>
       </c>
-      <c r="Z45" s="24">
+      <c r="Z45" s="20">
         <v>6</v>
       </c>
-      <c r="AA45" s="24">
+      <c r="AA45" s="20">
         <v>7</v>
       </c>
-      <c r="AB45" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="23">
+      <c r="AB45" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="19">
         <v>1</v>
       </c>
-      <c r="AD45" s="23">
+      <c r="AD45" s="19">
         <v>2</v>
       </c>
-      <c r="AE45" s="23">
+      <c r="AE45" s="19">
         <v>3</v>
       </c>
-      <c r="AF45" s="24">
+      <c r="AF45" s="20">
         <v>4</v>
       </c>
-      <c r="AG45" s="24">
+      <c r="AG45" s="20">
         <v>5</v>
       </c>
-      <c r="AH45" s="24">
+      <c r="AH45" s="20">
         <v>6</v>
       </c>
-      <c r="AI45" s="24">
+      <c r="AI45" s="20">
         <v>7</v>
       </c>
     </row>
@@ -1839,12 +1842,114 @@
       <c r="M48">
         <v>14</v>
       </c>
-      <c r="P48" t="s">
+    </row>
+    <row r="49" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L49" t="s">
         <v>59</v>
       </c>
+      <c r="M49">
+        <f>_xlfn.FLOOR.MATH(M48/8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L50" t="s">
+        <v>60</v>
+      </c>
+      <c r="M50">
+        <f>MOD(M48,8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L52" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="22"/>
+      <c r="S52" s="23"/>
+    </row>
+    <row r="53" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L53" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
+    </row>
+    <row r="54" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L54" s="19">
+        <v>0</v>
+      </c>
+      <c r="M54" s="19">
+        <v>1</v>
+      </c>
+      <c r="N54" s="19">
+        <v>2</v>
+      </c>
+      <c r="O54" s="19">
+        <v>3</v>
+      </c>
+      <c r="P54" s="20">
+        <v>4</v>
+      </c>
+      <c r="Q54" s="20">
+        <v>5</v>
+      </c>
+      <c r="R54" s="20">
+        <v>6</v>
+      </c>
+      <c r="S54" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L55" s="9">
+        <v>8</v>
+      </c>
+      <c r="M55" s="9">
+        <v>9</v>
+      </c>
+      <c r="N55" s="9">
+        <v>10</v>
+      </c>
+      <c r="O55" s="9">
+        <v>11</v>
+      </c>
+      <c r="P55" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q55" s="9">
+        <v>13</v>
+      </c>
+      <c r="R55" s="9">
+        <v>14</v>
+      </c>
+      <c r="S55" s="9">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="L52:S52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="P27:S27"/>
+    <mergeCell ref="T27:W27"/>
     <mergeCell ref="AB43:AI43"/>
     <mergeCell ref="AB44:AE44"/>
     <mergeCell ref="AF44:AI44"/>
@@ -1857,11 +1962,6 @@
     <mergeCell ref="P44:S44"/>
     <mergeCell ref="T44:W44"/>
     <mergeCell ref="X44:AA44"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="P27:S27"/>
-    <mergeCell ref="T27:W27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cosmetic variable name change
</commit_message>
<xml_diff>
--- a/Docs/Other/sprite_bounds_check.xlsx
+++ b/Docs/Other/sprite_bounds_check.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>temp</t>
   </si>
@@ -207,13 +207,28 @@
   </si>
   <si>
     <t>x%8</t>
+  </si>
+  <si>
+    <t>get x</t>
+  </si>
+  <si>
+    <t>get tile</t>
+  </si>
+  <si>
+    <t>get pixel</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>tmptr + tile#*2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,8 +245,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +311,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -480,6 +508,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -813,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI55"/>
+  <dimension ref="A1:AI60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X58" sqref="X58"/>
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:27" x14ac:dyDescent="0.25">
       <c r="L49" t="s">
         <v>59</v>
       </c>
@@ -1852,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="12:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:27" x14ac:dyDescent="0.25">
       <c r="L50" t="s">
         <v>60</v>
       </c>
@@ -1861,8 +1892,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="12:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L52" s="21" t="s">
         <v>53</v>
       </c>
@@ -1873,8 +1904,18 @@
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
       <c r="S52" s="23"/>
-    </row>
-    <row r="53" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T52" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="U52" s="22"/>
+      <c r="V52" s="22"/>
+      <c r="W52" s="22"/>
+      <c r="X52" s="22"/>
+      <c r="Y52" s="22"/>
+      <c r="Z52" s="22"/>
+      <c r="AA52" s="23"/>
+    </row>
+    <row r="53" spans="12:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L53" s="24" t="s">
         <v>50</v>
       </c>
@@ -1887,8 +1928,20 @@
       <c r="Q53" s="25"/>
       <c r="R53" s="25"/>
       <c r="S53" s="26"/>
-    </row>
-    <row r="54" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="U53" s="25"/>
+      <c r="V53" s="25"/>
+      <c r="W53" s="26"/>
+      <c r="X53" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y53" s="25"/>
+      <c r="Z53" s="25"/>
+      <c r="AA53" s="26"/>
+    </row>
+    <row r="54" spans="12:27" x14ac:dyDescent="0.25">
       <c r="L54" s="19">
         <v>0</v>
       </c>
@@ -1913,8 +1966,32 @@
       <c r="S54" s="20">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="19">
+        <v>0</v>
+      </c>
+      <c r="U54" s="19">
+        <v>1</v>
+      </c>
+      <c r="V54" s="19">
+        <v>2</v>
+      </c>
+      <c r="W54" s="19">
+        <v>3</v>
+      </c>
+      <c r="X54" s="20">
+        <v>4</v>
+      </c>
+      <c r="Y54" s="20">
+        <v>5</v>
+      </c>
+      <c r="Z54" s="20">
+        <v>6</v>
+      </c>
+      <c r="AA54" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="12:27" x14ac:dyDescent="0.25">
       <c r="L55" s="9">
         <v>8</v>
       </c>
@@ -1933,22 +2010,63 @@
       <c r="Q55" s="9">
         <v>13</v>
       </c>
-      <c r="R55" s="9">
+      <c r="R55" s="28">
         <v>14</v>
       </c>
-      <c r="S55" s="9">
+      <c r="S55" s="28">
         <v>15</v>
       </c>
+      <c r="T55" s="28">
+        <v>16</v>
+      </c>
+      <c r="U55" s="28">
+        <v>17</v>
+      </c>
+      <c r="V55" s="28">
+        <v>18</v>
+      </c>
+      <c r="W55" s="28">
+        <v>19</v>
+      </c>
+      <c r="X55" s="28">
+        <v>20</v>
+      </c>
+      <c r="Y55" s="28">
+        <v>21</v>
+      </c>
+      <c r="Z55" s="9">
+        <v>22</v>
+      </c>
+      <c r="AA55" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L59" t="s">
+        <v>62</v>
+      </c>
+      <c r="M59" t="s">
+        <v>64</v>
+      </c>
+      <c r="N59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="L52:S52"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="P53:S53"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="P27:S27"/>
+  <mergeCells count="23">
+    <mergeCell ref="T52:AA52"/>
+    <mergeCell ref="T53:W53"/>
+    <mergeCell ref="X53:AA53"/>
     <mergeCell ref="T27:W27"/>
     <mergeCell ref="AB43:AI43"/>
     <mergeCell ref="AB44:AE44"/>
@@ -1962,6 +2080,13 @@
     <mergeCell ref="P44:S44"/>
     <mergeCell ref="T44:W44"/>
     <mergeCell ref="X44:AA44"/>
+    <mergeCell ref="L52:S52"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="P27:S27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>